<commit_message>
penulisan dokumentasi todo list v1 excel selesai
</commit_message>
<xml_diff>
--- a/erd_n_features/Features.xlsx
+++ b/erd_n_features/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\tryLaravel\todo-list\erd_n_features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4449604-4D23-449E-AEF0-7AF2C341AE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE00A9E-C455-4ABC-AB26-1A4010159AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{5F6D916F-4321-4B50-A99F-3ABAB18A779B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{5F6D916F-4321-4B50-A99F-3ABAB18A779B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringkasan Aplikasi" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
   <si>
     <t>Role</t>
   </si>
@@ -334,6 +334,62 @@
   </si>
   <si>
     <t>Halaman untuk memperbarui / mengubah data penugasan.</t>
+  </si>
+  <si>
+    <t>Mengubah data penugasan dari nama tugas, waktu mulai/selesai, pelaksana. Terdapat dua tombol simpan pembaruan dan tombol beranda</t>
+  </si>
+  <si>
+    <t>Terdapat tiga tombol kembali ke beranda, data penugasan dan tombol data pegawai ( halaman saat ini ).</t>
+  </si>
+  <si>
+    <t>Tugas Saya</t>
+  </si>
+  <si>
+    <t>Halaman menampilkan tugas yang diberikan khusus sesuai akun manajer.</t>
+  </si>
+  <si>
+    <t>Terdapat tombol kembali ke beranda. Dan dua tombol lain untuk mengubah penugasan dan menghapus tugas.</t>
+  </si>
+  <si>
+    <t>Detail Tugas</t>
+  </si>
+  <si>
+    <t>Menampilkan data lengkap tugas yang diberikan admin/manajer.</t>
+  </si>
+  <si>
+    <t>Hanya memiliki fitur pengubahan untuk status tugas "Ditolak"/"Selesai". Memiliki sebuah tombol menyimpan pembaruan dan empat tombol lain untuk akses ke beranda, penugasa ( halaman sekarang ), tugas selesai/ditolak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terdapat tombol untuk kembali ke beranda, penugasan selesai ( halaman sekarang ), tugas selesai/ditolak.dan melihat penugasan yang selesai oleh pegawai. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terdapat tombol untuk kembali ke beranda, penugasan ditolak ( halaman sekarang ), tugas selesai/ditolak.dan melihat penugasan yang tidak selesai oleh pegawai. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Terdapat menu Penugasan, Daftar Tugas, Tugas Selesai, Tugas Ditolak, button profil dan keluar ( </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> )</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -409,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,6 +513,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,13 +526,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -864,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFA20E4-7AE7-44D2-8776-6AF41F65594F}">
   <dimension ref="A4:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -902,7 +961,7 @@
       <c r="C5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="3"/>
@@ -932,7 +991,7 @@
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="3"/>
@@ -955,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4936F9-4A98-46C5-8C98-AA044BFBE17B}">
   <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1137,27 +1196,27 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="3"/>
@@ -1222,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089FC60C-1BE8-430C-8617-EBE7E5D0BB71}">
   <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1328,47 +1387,71 @@
       <c r="D8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E8" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="C12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B13" s="1">
-        <v>11</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,15 +1461,134 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DD306D-D0A0-4087-9A1A-8A74513B4A31}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="13.1328125" customWidth="1"/>
+    <col min="4" max="4" width="34.46484375" customWidth="1"/>
+    <col min="5" max="5" width="53.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>